<commit_message>
big fix custom copy
</commit_message>
<xml_diff>
--- a/system_template/data/mail_template.xlsx
+++ b/system_template/data/mail_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dropbox\3_Develop\TFS_Exc\ExmentProject\vendor\exceedone\exment\system_template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F26BE5B8-8F18-4DDE-AF89-AB99ADD388E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB01F296-2E75-463C-9FDB-8E237ECC6744}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Bug fix notify user name
</commit_message>
<xml_diff>
--- a/system_template/data/mail_template.xlsx
+++ b/system_template/data/mail_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dropbox\3_Develop\TFS_Exc\ExmentProject\vendor\exceedone\exment\system_template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE1FBD7-9C4C-4C4E-86B1-7F78A909A4E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4686BFB2-0221-4318-93C0-26CF1EA25FB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
   <sheets>
     <sheet name="mail_template" sheetId="1" r:id="rId1"/>
@@ -721,7 +721,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>